<commit_message>
More updates to the script
</commit_message>
<xml_diff>
--- a/Inputs/Thrasio TikTok Shop-Campaign Report(2024-05-12 to 2024-05-18).xlsx
+++ b/Inputs/Thrasio TikTok Shop-Campaign Report(2024-05-12 to 2024-05-18).xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/261a4915364edc4c/Coding/Projects/Tiktok Weekly Process/Inputs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_D746C4AF3C503E2BFC5F3B65A32805E66EC0E939" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A455E136-CA37-40F2-BAF0-40F08C576651}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="35">
   <si>
     <t>Campaign name</t>
   </si>
@@ -124,11 +130,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.00%"/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,20 +188,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -236,7 +247,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -270,6 +281,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -304,9 +316,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -479,14 +492,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,7 +554,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -586,7 +604,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -612,7 +630,7 @@
         <v>1763</v>
       </c>
       <c r="I3" s="2">
-        <v>0.0115</v>
+        <v>1.15E-2</v>
       </c>
       <c r="J3">
         <v>109</v>
@@ -621,7 +639,7 @@
         <v>22.98</v>
       </c>
       <c r="L3" s="2">
-        <v>0.0007000000000000001</v>
+        <v>7.000000000000001E-4</v>
       </c>
       <c r="M3" t="s">
         <v>33</v>
@@ -636,7 +654,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -647,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>4420.23</v>
+        <v>4420.2299999999996</v>
       </c>
       <c r="E4">
         <v>1.54</v>
@@ -662,7 +680,7 @@
         <v>2877</v>
       </c>
       <c r="I4" s="2">
-        <v>0.0135</v>
+        <v>1.35E-2</v>
       </c>
       <c r="J4">
         <v>262</v>
@@ -671,7 +689,7 @@
         <v>16.87</v>
       </c>
       <c r="L4" s="2">
-        <v>0.0012</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="M4" t="s">
         <v>33</v>
@@ -686,7 +704,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -736,7 +754,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -747,13 +765,13 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>885.4400000000001</v>
+        <v>885.44</v>
       </c>
       <c r="E6">
-        <v>2.22</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="F6">
-        <v>16.15</v>
+        <v>16.149999999999999</v>
       </c>
       <c r="G6">
         <v>54837</v>
@@ -762,7 +780,7 @@
         <v>399</v>
       </c>
       <c r="I6" s="2">
-        <v>0.0073</v>
+        <v>7.3000000000000001E-3</v>
       </c>
       <c r="J6">
         <v>88</v>
@@ -771,7 +789,7 @@
         <v>10.06</v>
       </c>
       <c r="L6" s="2">
-        <v>0.0016</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="M6" t="s">
         <v>33</v>
@@ -786,7 +804,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -836,7 +854,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -850,10 +868,10 @@
         <v>6923.07</v>
       </c>
       <c r="E8">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="F8">
-        <v>16.01</v>
+        <v>16.010000000000002</v>
       </c>
       <c r="G8">
         <v>432465</v>
@@ -862,16 +880,16 @@
         <v>10046</v>
       </c>
       <c r="I8" s="2">
-        <v>0.0232</v>
+        <v>2.3199999999999998E-2</v>
       </c>
       <c r="J8">
         <v>383</v>
       </c>
       <c r="K8">
-        <v>18.08</v>
+        <v>18.079999999999998</v>
       </c>
       <c r="L8" s="2">
-        <v>0.0009</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="M8" t="s">
         <v>33</v>
@@ -886,7 +904,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -912,7 +930,7 @@
         <v>3209</v>
       </c>
       <c r="I9" s="2">
-        <v>0.0166</v>
+        <v>1.66E-2</v>
       </c>
       <c r="J9">
         <v>471</v>
@@ -921,7 +939,7 @@
         <v>6.1</v>
       </c>
       <c r="L9" s="2">
-        <v>0.0024</v>
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="M9" t="s">
         <v>33</v>
@@ -936,7 +954,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -986,7 +1004,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1036,7 +1054,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1086,7 +1104,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1136,7 +1154,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1186,7 +1204,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1212,16 +1230,16 @@
         <v>643</v>
       </c>
       <c r="I15" s="2">
-        <v>0.0066</v>
+        <v>6.6E-3</v>
       </c>
       <c r="J15">
         <v>54</v>
       </c>
       <c r="K15">
-        <v>36.16</v>
+        <v>36.159999999999997</v>
       </c>
       <c r="L15" s="2">
-        <v>0.0005999999999999999</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="M15" t="s">
         <v>33</v>
@@ -1236,7 +1254,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1253,7 +1271,7 @@
         <v>1.03</v>
       </c>
       <c r="F16">
-        <v>17.1</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="G16">
         <v>1143951</v>
@@ -1262,7 +1280,7 @@
         <v>18937</v>
       </c>
       <c r="I16" s="2">
-        <v>0.0166</v>
+        <v>1.66E-2</v>
       </c>
       <c r="J16">
         <v>1367</v>
@@ -1271,7 +1289,7 @@
         <v>14.31</v>
       </c>
       <c r="L16" s="2">
-        <v>0.0012</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="M16" t="s">
         <v>33</v>

</xml_diff>